<commit_message>
New parser and modified get_criteria
</commit_message>
<xml_diff>
--- a/graphe_problems.xlsx
+++ b/graphe_problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taogr\Documents\M2DSC\MAS\MAP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48773EE9-71AF-4284-A9A8-035FA5A5A2F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF313CF6-5A3A-4980-A3C6-97C3565BFE06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Execution time</t>
-  </si>
-  <si>
     <t>Size of information</t>
   </si>
   <si>
@@ -51,10 +48,16 @@
     <t>DSA</t>
   </si>
   <si>
-    <t>88,488 ms</t>
-  </si>
-  <si>
-    <t>28,718 ms</t>
+    <t>scen05</t>
+  </si>
+  <si>
+    <t>Execution time (in ms)</t>
+  </si>
+  <si>
+    <t>Max frequency</t>
+  </si>
+  <si>
+    <t>Number of different frequency</t>
   </si>
 </sst>
 </file>
@@ -373,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -385,34 +388,42 @@
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="25.21875" customWidth="1"/>
     <col min="5" max="5" width="17.77734375" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="27.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
+      <c r="C2" s="1">
+        <v>28718</v>
       </c>
       <c r="D2" s="1">
         <v>988000</v>
@@ -420,22 +431,80 @@
       <c r="E2" s="1">
         <v>20806499</v>
       </c>
+      <c r="F2" s="1">
+        <v>792</v>
+      </c>
+      <c r="G2" s="1">
+        <v>44</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>88488</v>
       </c>
       <c r="D3" s="1">
         <v>491530</v>
       </c>
       <c r="E3" s="1">
         <v>10355110</v>
+      </c>
+      <c r="F3">
+        <v>792</v>
+      </c>
+      <c r="G3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>25250</v>
+      </c>
+      <c r="D4">
+        <v>2078400</v>
+      </c>
+      <c r="E4">
+        <v>43627015</v>
+      </c>
+      <c r="F4">
+        <v>792</v>
+      </c>
+      <c r="G4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>26341</v>
+      </c>
+      <c r="D5">
+        <v>1034004</v>
+      </c>
+      <c r="E5">
+        <v>21771879</v>
+      </c>
+      <c r="F5">
+        <v>792</v>
+      </c>
+      <c r="G5">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New results and updated Excel
</commit_message>
<xml_diff>
--- a/graphe_problems.xlsx
+++ b/graphe_problems.xlsx
@@ -10,6 +10,9 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Feuil1!$A$1:$G$20</definedName>
+  </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="18">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -43,28 +46,34 @@
     <t xml:space="preserve">Max frequency</t>
   </si>
   <si>
+    <t xml:space="preserve">ADOPT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scen00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DPOP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaxSum</t>
+  </si>
+  <si>
     <t xml:space="preserve">MGM</t>
   </si>
   <si>
     <t xml:space="preserve">scen02</t>
   </si>
   <si>
-    <t xml:space="preserve">DSA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MaxSum</t>
-  </si>
-  <si>
     <t xml:space="preserve">scen03</t>
   </si>
   <si>
-    <t xml:space="preserve">ADOPT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scen00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DPOP</t>
+    <t xml:space="preserve">scen05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scen06</t>
   </si>
   <si>
     <t xml:space="preserve">scen12</t>
@@ -102,18 +111,12 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEF413D"/>
-        <bgColor rgb="FF993366"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -150,20 +153,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -176,67 +175,11 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFEF413D"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -244,10 +187,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -263,25 +206,25 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -292,43 +235,31 @@
       <c r="B2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="n">
-        <v>37276</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>988000</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>30911212</v>
-      </c>
-      <c r="F2" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="G2" s="1" t="n">
-        <v>792</v>
+      <c r="C2" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>54</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>7287</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="n">
-        <v>88488</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>491530</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>10355110</v>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v>44</v>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>792</v>
+      <c r="C3" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>5691</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -339,42 +270,30 @@
         <v>8</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>9616</v>
+        <v>95</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>3745</v>
+        <v>1194</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>2554910</v>
-      </c>
-      <c r="F4" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G4" s="0" t="n">
-        <v>792</v>
+        <v>25130</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>70025</v>
+        <v>32</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>2208000</v>
+        <v>14</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>69080908</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>792</v>
+        <v>3909</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -382,67 +301,79 @@
         <v>12</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>37</v>
+        <v>91</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>54</v>
+        <v>2400</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>7287</v>
+        <v>54461</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>36</v>
+        <v>45060</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>24</v>
+        <v>491530</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>5691</v>
+        <v>10376474</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>95</v>
+        <v>9616</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>1194</v>
+        <v>3745</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>25130</v>
+        <v>2554910</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>792</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="0" t="n">
-        <v>91</v>
-      </c>
-      <c r="D9" s="0" t="n">
-        <v>2400</v>
-      </c>
-      <c r="E9" s="0" t="n">
-        <v>54461</v>
+      <c r="C9" s="2" t="n">
+        <v>37276</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>988000</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>30911212</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>44</v>
+      </c>
+      <c r="G9" s="2" t="n">
+        <v>792</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -450,24 +381,30 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="0" t="n">
-        <v>32</v>
+        <v>71054</v>
       </c>
       <c r="D10" s="0" t="n">
-        <v>14</v>
+        <v>1098480</v>
       </c>
       <c r="E10" s="0" t="n">
-        <v>3909</v>
+        <v>23184086</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>46</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>792</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>14672</v>
@@ -487,19 +424,19 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C12" s="0" t="n">
-        <v>71054</v>
+        <v>70025</v>
       </c>
       <c r="D12" s="0" t="n">
-        <v>1098480</v>
+        <v>2208000</v>
       </c>
       <c r="E12" s="0" t="n">
-        <v>23184086</v>
+        <v>69080908</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>46</v>
@@ -510,53 +447,53 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>2071</v>
+        <v>73729</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>17910</v>
+        <v>1034004</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>377298</v>
+        <v>21846827</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>3382</v>
+        <v>60913</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>804</v>
+        <v>2078400</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>232590</v>
+        <v>65038702</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>1968</v>
+        <v>35608</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>36000</v>
+        <v>526156</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>1125684</v>
+        <v>11093401</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -564,19 +501,88 @@
         <v>12</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C16" s="0" t="n">
+        <v>45186</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>1057600</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>33086550</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="0" t="n">
         <v>1831016</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D17" s="0" t="n">
         <v>96199</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E17" s="0" t="n">
         <v>6765370</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>2071</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>17910</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>377298</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>3382</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>804</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <v>232590</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>1968</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>36000</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <v>1125684</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:G20"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -584,5 +590,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>